<commit_message>
KARMEN-3 ALGORITHM IN LIPIDS CHANGED
</commit_message>
<xml_diff>
--- a/analyst/Ines/rmonize/data_proc_elem/DPE_KARMEN_INES.xlsx
+++ b/analyst/Ines/rmonize/data_proc_elem/DPE_KARMEN_INES.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perrar\Documents\Perrar\NFDI4Health\TA5_1\use-cases-harmonisation\analyst\Ines\rmonize\data_proc_elem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\analyst\Ines\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7913EEA9-3D69-408B-A550-E9222060E2EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -273,9 +274,6 @@
     <t>operation</t>
   </si>
   <si>
-    <t>KL_TG * 88.57</t>
-  </si>
-  <si>
     <t>complete</t>
   </si>
   <si>
@@ -285,21 +283,12 @@
     <t>KL_CHO</t>
   </si>
   <si>
-    <t>KL_CHO * 38.67</t>
-  </si>
-  <si>
     <t>KL_LDLC</t>
   </si>
   <si>
-    <t>KL_LDLC * 38.67</t>
-  </si>
-  <si>
     <t>KL_HDLC</t>
   </si>
   <si>
-    <t>KL_HDLC * 38.67</t>
-  </si>
-  <si>
     <t>kcal_zb_tag_NCI</t>
   </si>
   <si>
@@ -370,12 +359,24 @@
   </si>
   <si>
     <t>KMF_tag_NCI</t>
+  </si>
+  <si>
+    <t>KL_CHO * 0.0259</t>
+  </si>
+  <si>
+    <t>KL_LDLC * 0.0259</t>
+  </si>
+  <si>
+    <t>KL_HDLC * 0.0259</t>
+  </si>
+  <si>
+    <t>KL_TG * 0.0113</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -462,7 +463,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -478,7 +479,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -553,6 +554,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -588,6 +606,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -763,20 +798,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B18" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="50.54296875" customWidth="1"/>
-    <col min="5" max="5" width="15.7265625" customWidth="1"/>
+    <col min="3" max="3" width="50.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="14.26953125" customWidth="1"/>
-    <col min="8" max="8" width="15.7265625" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1">
@@ -825,7 +860,7 @@
         <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>82</v>
@@ -834,14 +869,14 @@
         <v>83</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>84</v>
+        <v>116</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>86</v>
       </c>
       <c r="L2" s="2"/>
     </row>
@@ -856,23 +891,23 @@
         <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>83</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>86</v>
       </c>
       <c r="L3" s="2"/>
     </row>
@@ -887,23 +922,23 @@
         <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>83</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>86</v>
       </c>
       <c r="L4" s="2"/>
     </row>
@@ -918,23 +953,23 @@
         <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>83</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>92</v>
+        <v>115</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K5" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>86</v>
       </c>
       <c r="L5" s="2"/>
     </row>
@@ -949,23 +984,23 @@
         <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>11</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="L6" s="2"/>
     </row>
@@ -980,21 +1015,21 @@
         <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1008,23 +1043,23 @@
         <v>13</v>
       </c>
       <c r="E8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="I8" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="H8" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>108</v>
-      </c>
       <c r="J8" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1038,23 +1073,23 @@
         <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="I9" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="H9" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>108</v>
-      </c>
       <c r="J9" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1068,21 +1103,21 @@
         <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="8" customFormat="1">
@@ -1096,22 +1131,22 @@
         <v>13</v>
       </c>
       <c r="E11" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:12" s="8" customFormat="1">
@@ -1125,19 +1160,19 @@
         <v>13</v>
       </c>
       <c r="E12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1151,21 +1186,21 @@
         <v>13</v>
       </c>
       <c r="E13" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:12" s="5" customFormat="1">
@@ -1180,21 +1215,21 @@
         <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="I14" s="6"/>
       <c r="J14" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1209,23 +1244,23 @@
         <v>13</v>
       </c>
       <c r="E15" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>40</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I15" s="6"/>
       <c r="J15" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:12" s="5" customFormat="1">
@@ -1240,21 +1275,21 @@
         <v>13</v>
       </c>
       <c r="E16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="I16" s="6"/>
       <c r="J16" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="2:11" s="8" customFormat="1">
@@ -1268,22 +1303,22 @@
         <v>13</v>
       </c>
       <c r="E17" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="2:11">
@@ -1297,23 +1332,23 @@
         <v>13</v>
       </c>
       <c r="E18" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I18" s="6"/>
       <c r="J18" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="2:11">
@@ -1327,22 +1362,22 @@
         <v>13</v>
       </c>
       <c r="E19" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F19" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="G19" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K19" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="2:11">
@@ -1356,22 +1391,22 @@
         <v>13</v>
       </c>
       <c r="E20" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F20" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G20" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K20" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="2:11">
@@ -1385,22 +1420,22 @@
         <v>13</v>
       </c>
       <c r="E21" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F21" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="G21" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K21" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="2:11">
@@ -1414,22 +1449,22 @@
         <v>13</v>
       </c>
       <c r="E22" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F22" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G22" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K22" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="2:11">
@@ -1443,22 +1478,22 @@
         <v>13</v>
       </c>
       <c r="E23" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F23" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G23" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K23" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="2:11">
@@ -1472,22 +1507,22 @@
         <v>13</v>
       </c>
       <c r="E24" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F24" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G24" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K24" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="2:11">
@@ -1501,22 +1536,22 @@
         <v>13</v>
       </c>
       <c r="E25" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F25" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="G25" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K25" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="2:11">
@@ -1530,22 +1565,22 @@
         <v>13</v>
       </c>
       <c r="E26" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F26" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G26" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K26" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="2:11">
@@ -1559,22 +1594,22 @@
         <v>13</v>
       </c>
       <c r="E27" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F27" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G27" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K27" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="2:11" s="8" customFormat="1">
@@ -1588,22 +1623,22 @@
         <v>13</v>
       </c>
       <c r="E28" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K28" s="8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="2:11">
@@ -1617,21 +1652,21 @@
         <v>13</v>
       </c>
       <c r="E29" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F29" s="6"/>
       <c r="G29" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="I29" s="6"/>
       <c r="J29" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="2:11">
@@ -1645,21 +1680,21 @@
         <v>13</v>
       </c>
       <c r="E30" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F30" s="6"/>
       <c r="G30" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="I30" s="6"/>
       <c r="J30" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="2:11">
@@ -1673,23 +1708,23 @@
         <v>13</v>
       </c>
       <c r="E31" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I31" s="6"/>
       <c r="J31" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K31" s="6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="2:11">
@@ -1703,23 +1738,23 @@
         <v>13</v>
       </c>
       <c r="E32" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I32" s="6"/>
       <c r="J32" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K32" s="6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="2:11">
@@ -1733,21 +1768,21 @@
         <v>13</v>
       </c>
       <c r="E33" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F33" s="6"/>
       <c r="G33" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="I33" s="6"/>
       <c r="J33" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="K33" s="6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="2:11">
@@ -1761,21 +1796,21 @@
         <v>13</v>
       </c>
       <c r="E34" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F34" s="6"/>
       <c r="G34" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="I34" s="6"/>
       <c r="J34" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="K34" s="6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="2:11">
@@ -1789,23 +1824,23 @@
         <v>13</v>
       </c>
       <c r="E35" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I35" s="6"/>
       <c r="J35" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K35" s="6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="2:11">
@@ -1819,22 +1854,22 @@
         <v>13</v>
       </c>
       <c r="E36" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F36" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G36" s="6" t="s">
         <v>83</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K36" s="6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>